<commit_message>
Proceso de Busqieda de Personas
</commit_message>
<xml_diff>
--- a/UtilidadesAmigos.Solucion/Temporal/REQUERIMIENTOS 27.7.2021.xlsx
+++ b/UtilidadesAmigos.Solucion/Temporal/REQUERIMIENTOS 27.7.2021.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ing. Juan Medina\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{AECDFBF0-BEDD-469F-87DC-8B48CC30E0D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{1843679C-FEC1-4A07-AA14-D3CE3CDECD54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,8 +17,8 @@
   </sheets>
   <calcPr calcId="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Dilcia Urena - Vista personalizada" guid="{CB9DB39E-62B3-45A4-AFB8-BFA1B88B5C14}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="1"/>
     <customWorkbookView name="Ing. Juan Medina - Personal View" guid="{F0A1C4B5-5EEB-4B49-A06F-5A5BE0C7B926}" mergeInterval="0" personalView="1" maximized="1" xWindow="-9" yWindow="-9" windowWidth="1938" windowHeight="1038" activeSheetId="1"/>
-    <customWorkbookView name="Dilcia Urena - Vista personalizada" guid="{CB9DB39E-62B3-45A4-AFB8-BFA1B88B5C14}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="1"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -204,7 +204,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -242,6 +242,12 @@
       <sz val="10"/>
       <color rgb="FF212529"/>
       <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -338,7 +344,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -408,11 +414,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,7 +442,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{241E666E-0F8F-43D7-9F04-668D4A4AFEFD}" diskRevisions="1" revisionId="24" version="4">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{2A121355-4023-44F6-AF9E-6B75F56DCDC1}" diskRevisions="1" revisionId="24" version="5">
   <header guid="{2AA1DB6C-38D7-43D8-A80D-489977938259}" dateTime="2021-07-27T13:31:04" maxSheetId="2" userName="Dilcia Urena" r:id="rId1">
     <sheetIdMap count="1">
       <sheetId val="1"/>
@@ -463,6 +474,11 @@
     </sheetIdMap>
   </header>
   <header guid="{241E666E-0F8F-43D7-9F04-668D4A4AFEFD}" dateTime="2021-07-29T17:09:14" maxSheetId="2" userName="Ing. Juan Medina" r:id="rId7" minRId="21" maxRId="24">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{2A121355-4023-44F6-AF9E-6B75F56DCDC1}" dateTime="2021-08-06T09:32:33" maxSheetId="2" userName="Ing. Juan Medina" r:id="rId8">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
@@ -6773,6 +6789,18 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog8.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="1" sqref="A30:XFD30" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+  </rfmt>
+</revisions>
+</file>
+
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
 <users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="0"/>
 </file>
@@ -6977,8 +7005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:XFD30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
@@ -7040,13 +7068,13 @@
       <c r="A4" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="B4" s="29"/>
+      <c r="B4" s="27"/>
     </row>
     <row r="5" spans="1:24" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A5" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="B5" s="29"/>
+      <c r="B5" s="27"/>
     </row>
     <row r="6" spans="1:24" ht="15.75" customHeight="1">
       <c r="A6" s="4" t="s">
@@ -7758,35 +7786,13 @@
       <c r="W29" s="1"/>
       <c r="X29" s="1"/>
     </row>
-    <row r="30" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A30" s="10" t="s">
+    <row r="30" spans="1:24" s="32" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A30" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="B30" s="20" t="s">
+      <c r="B30" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-      <c r="K30" s="1"/>
-      <c r="L30" s="1"/>
-      <c r="M30" s="1"/>
-      <c r="N30" s="1"/>
-      <c r="O30" s="1"/>
-      <c r="P30" s="1"/>
-      <c r="Q30" s="1"/>
-      <c r="R30" s="1"/>
-      <c r="S30" s="1"/>
-      <c r="T30" s="1"/>
-      <c r="U30" s="1"/>
-      <c r="V30" s="1"/>
-      <c r="W30" s="1"/>
-      <c r="X30" s="1"/>
     </row>
     <row r="31" spans="1:24" ht="15.75" customHeight="1">
       <c r="A31" s="10" t="s">
@@ -8051,8 +8057,8 @@
       <c r="X39" s="1"/>
     </row>
     <row r="40" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A40" s="27"/>
-      <c r="B40" s="28"/>
+      <c r="A40" s="28"/>
+      <c r="B40" s="29"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
@@ -32300,13 +32306,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{F0A1C4B5-5EEB-4B49-A06F-5A5BE0C7B926}">
-      <selection activeCell="A17" sqref="A17"/>
+    <customSheetView guid="{CB9DB39E-62B3-45A4-AFB8-BFA1B88B5C14}">
+      <selection sqref="A1:D1"/>
       <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0" footer="0"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
-    <customSheetView guid="{CB9DB39E-62B3-45A4-AFB8-BFA1B88B5C14}">
-      <selection sqref="A1:D1"/>
+    <customSheetView guid="{F0A1C4B5-5EEB-4B49-A06F-5A5BE0C7B926}">
+      <selection activeCell="A17" sqref="A17"/>
       <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0" footer="0"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
@@ -32315,6 +32321,6 @@
     <mergeCell ref="A40:B40"/>
   </mergeCells>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>